<commit_message>
BEIS end dates checked
End dates suppressed if past for an active project
</commit_message>
<xml_diff>
--- a/Inputs/BEIS_NF_MODARI_Q1_2021-2022.xlsx
+++ b/Inputs/BEIS_NF_MODARI_Q1_2021-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wellcomecloud-my.sharepoint.com/personal/e_clegg_ukcds_org_uk/Documents/My Documents/GitHub/ODA_research_and_innovation/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{9033F106-F950-4DDA-AA21-D7458A76853E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{BDB85B13-C4A7-49E3-8439-D8756ADCFF59}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{9033F106-F950-4DDA-AA21-D7458A76853E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{C03FE914-FF74-4661-BFCF-7942D945330D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A27C8570-391C-4382-B6BE-58C490CED2C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6228" uniqueCount="1480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6226" uniqueCount="1480">
   <si>
     <t>Recipient region</t>
   </si>
@@ -4561,7 +4561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -4569,6 +4569,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4885,7 +4886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFA6D71-3537-44AE-A362-E4817137C587}">
   <dimension ref="A1:L618"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4960,8 +4963,8 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>59</v>
+      <c r="G2" s="7">
+        <v>42186</v>
       </c>
       <c r="H2" t="s">
         <v>59</v>
@@ -4998,8 +5001,8 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>50</v>
+      <c r="G3" s="7">
+        <v>42005</v>
       </c>
       <c r="H3" t="s">
         <v>50</v>
@@ -26677,5 +26680,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>